<commit_message>
final tumor volume measurements
</commit_message>
<xml_diff>
--- a/data/tumor-size/AOT00048953-mimic15/AOT00048953-mimic15_tumor-size.xlsx
+++ b/data/tumor-size/AOT00048953-mimic15/AOT00048953-mimic15_tumor-size.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://osumc-my.sharepoint.com/personal/wil407_osumc_edu/Documents/BuckeyeBox Data/mimic/data/AOT00048953-mimic15/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="251" documentId="14_{080B9E44-4A56-4BC6-8BED-9A1C81A62781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09D84013-DADD-4698-A4CE-7A1B36CD1C1C}"/>
+  <xr:revisionPtr revIDLastSave="469" documentId="14_{080B9E44-4A56-4BC6-8BED-9A1C81A62781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B19A594-C0DD-4EE0-ACDD-0B1593E17EF5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F3D21AEE-9DE9-46E2-BA29-C20A4AF54E28}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="14">
   <si>
     <t>date</t>
   </si>
@@ -65,9 +65,6 @@
     <t>tumor.width.(mm)</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Antibiotics</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Anti-PD1</t>
+  </si>
+  <si>
+    <t>Tumor.weight (g)</t>
   </si>
 </sst>
 </file>
@@ -439,11 +439,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7107C64-40D4-45F3-A949-3D4433E51656}">
-  <dimension ref="A1:K200"/>
+  <dimension ref="A1:K249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L179" sqref="L179"/>
+      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R243" sqref="R243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -488,7 +488,7 @@
         <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -544,7 +544,7 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5">
         <v>21.5</v>
@@ -561,7 +561,7 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6">
         <v>21.9</v>
@@ -578,7 +578,7 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7">
         <v>23</v>
@@ -637,7 +637,7 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11">
         <v>21.1</v>
@@ -654,7 +654,7 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G12">
         <v>23.1</v>
@@ -671,7 +671,7 @@
         <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G13">
         <v>23.7</v>
@@ -730,7 +730,7 @@
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17">
         <v>23.1</v>
@@ -747,7 +747,7 @@
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G18">
         <v>20.6</v>
@@ -764,7 +764,7 @@
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G19">
         <v>22.4</v>
@@ -823,7 +823,7 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G23">
         <v>23.4</v>
@@ -840,7 +840,7 @@
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G24">
         <v>22.3</v>
@@ -857,7 +857,7 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G25">
         <v>21.4</v>
@@ -916,7 +916,7 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G29">
         <v>25.7</v>
@@ -933,7 +933,7 @@
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G30">
         <v>25.2</v>
@@ -950,7 +950,7 @@
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G31">
         <v>25.4</v>
@@ -1009,7 +1009,7 @@
         <v>4</v>
       </c>
       <c r="E35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G35">
         <v>23.7</v>
@@ -1026,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="E36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G36">
         <v>24.9</v>
@@ -1043,7 +1043,7 @@
         <v>4</v>
       </c>
       <c r="E37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G37">
         <v>24.2</v>
@@ -1102,7 +1102,7 @@
         <v>6</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G41">
         <v>24.9</v>
@@ -1119,7 +1119,7 @@
         <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G42">
         <v>24.4</v>
@@ -1136,7 +1136,7 @@
         <v>6</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G43">
         <v>22.7</v>
@@ -1192,7 +1192,7 @@
         <v>8</v>
       </c>
       <c r="E47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G47">
         <v>25.8</v>
@@ -1209,7 +1209,7 @@
         <v>8</v>
       </c>
       <c r="E48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G48">
         <v>25</v>
@@ -1226,7 +1226,7 @@
         <v>8</v>
       </c>
       <c r="E49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -1300,7 +1300,7 @@
         <v>2</v>
       </c>
       <c r="E53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -1323,7 +1323,7 @@
         <v>2</v>
       </c>
       <c r="E54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H54">
         <v>1</v>
@@ -1346,7 +1346,7 @@
         <v>2</v>
       </c>
       <c r="E55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H55">
         <v>1</v>
@@ -1429,7 +1429,7 @@
         <v>4</v>
       </c>
       <c r="E59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -1452,7 +1452,7 @@
         <v>4</v>
       </c>
       <c r="E60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H60">
         <v>1</v>
@@ -1475,7 +1475,7 @@
         <v>4</v>
       </c>
       <c r="E61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H61">
         <v>1</v>
@@ -1558,7 +1558,7 @@
         <v>6</v>
       </c>
       <c r="E65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H65">
         <v>1</v>
@@ -1581,7 +1581,7 @@
         <v>6</v>
       </c>
       <c r="E66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H66">
         <v>1</v>
@@ -1604,7 +1604,7 @@
         <v>6</v>
       </c>
       <c r="E67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H67">
         <v>1</v>
@@ -1687,7 +1687,7 @@
         <v>8</v>
       </c>
       <c r="E71" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H71">
         <v>1</v>
@@ -1710,7 +1710,7 @@
         <v>8</v>
       </c>
       <c r="E72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H72">
         <v>1</v>
@@ -1733,7 +1733,7 @@
         <v>8</v>
       </c>
       <c r="E73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H73">
         <v>1</v>
@@ -1816,7 +1816,7 @@
         <v>2</v>
       </c>
       <c r="E77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H77">
         <v>1</v>
@@ -1839,7 +1839,7 @@
         <v>2</v>
       </c>
       <c r="E78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H78">
         <v>1</v>
@@ -1862,7 +1862,7 @@
         <v>2</v>
       </c>
       <c r="E79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H79">
         <v>1</v>
@@ -1945,7 +1945,7 @@
         <v>4</v>
       </c>
       <c r="E83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H83">
         <v>1</v>
@@ -1968,7 +1968,7 @@
         <v>4</v>
       </c>
       <c r="E84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H84">
         <v>1</v>
@@ -1991,7 +1991,7 @@
         <v>4</v>
       </c>
       <c r="E85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H85">
         <v>1</v>
@@ -2074,7 +2074,7 @@
         <v>6</v>
       </c>
       <c r="E89" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H89">
         <v>1</v>
@@ -2097,7 +2097,7 @@
         <v>6</v>
       </c>
       <c r="E90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H90">
         <v>1</v>
@@ -2120,7 +2120,7 @@
         <v>6</v>
       </c>
       <c r="E91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H91">
         <v>1</v>
@@ -2203,7 +2203,7 @@
         <v>8</v>
       </c>
       <c r="E95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H95">
         <v>1</v>
@@ -2226,7 +2226,7 @@
         <v>8</v>
       </c>
       <c r="E96" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H96">
         <v>1</v>
@@ -2249,7 +2249,7 @@
         <v>8</v>
       </c>
       <c r="E97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H97">
         <v>1</v>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="D101" s="3"/>
       <c r="E101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F101" s="3"/>
       <c r="G101" s="3">
@@ -2379,7 +2379,7 @@
       </c>
       <c r="D102" s="3"/>
       <c r="E102" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F102" s="3"/>
       <c r="G102" s="3">
@@ -2407,7 +2407,7 @@
       </c>
       <c r="D103" s="3"/>
       <c r="E103" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F103" s="3"/>
       <c r="G103" s="3">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="D107" s="3"/>
       <c r="E107" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F107" s="3"/>
       <c r="G107" s="3">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="D108" s="3"/>
       <c r="E108" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F108" s="3"/>
       <c r="G108" s="3">
@@ -2569,7 +2569,7 @@
       </c>
       <c r="D109" s="3"/>
       <c r="E109" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F109" s="3"/>
       <c r="G109" s="3">
@@ -2675,7 +2675,7 @@
       </c>
       <c r="D113" s="3"/>
       <c r="E113" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F113" s="3"/>
       <c r="G113" s="3">
@@ -2703,7 +2703,7 @@
       </c>
       <c r="D114" s="3"/>
       <c r="E114" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F114" s="3"/>
       <c r="G114" s="3">
@@ -2731,7 +2731,7 @@
       </c>
       <c r="D115" s="3"/>
       <c r="E115" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F115" s="3"/>
       <c r="G115" s="3">
@@ -2837,7 +2837,7 @@
       </c>
       <c r="D119" s="3"/>
       <c r="E119" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F119" s="3"/>
       <c r="G119" s="3">
@@ -2865,7 +2865,7 @@
       </c>
       <c r="D120" s="3"/>
       <c r="E120" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F120" s="3"/>
       <c r="G120" s="3">
@@ -2893,7 +2893,7 @@
       </c>
       <c r="D121" s="3"/>
       <c r="E121" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F121" s="3"/>
       <c r="G121" s="3">
@@ -2920,7 +2920,7 @@
         <v>1</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E122" s="3"/>
       <c r="H122" s="3">
@@ -2944,7 +2944,7 @@
         <v>1</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E123" s="3"/>
       <c r="H123" s="3">
@@ -2968,7 +2968,7 @@
         <v>1</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E124" s="3"/>
       <c r="H124" s="3">
@@ -2992,10 +2992,10 @@
         <v>2</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E125" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H125" s="3">
         <v>1</v>
@@ -3018,10 +3018,10 @@
         <v>2</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E126" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H126" s="3">
         <v>1</v>
@@ -3044,10 +3044,10 @@
         <v>2</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E127" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H127" s="3">
         <v>1</v>
@@ -3070,10 +3070,10 @@
         <v>2</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E128" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H128" s="3">
         <v>2</v>
@@ -3096,7 +3096,7 @@
         <v>3</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E129" s="3"/>
       <c r="H129" s="3">
@@ -3120,7 +3120,7 @@
         <v>3</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E130" s="3"/>
       <c r="H130" s="3">
@@ -3144,7 +3144,7 @@
         <v>3</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E131" s="3"/>
       <c r="H131" s="3">
@@ -3168,10 +3168,10 @@
         <v>4</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E132" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H132" s="3">
         <v>1</v>
@@ -3194,10 +3194,10 @@
         <v>4</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E133" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H133" s="3">
         <v>1</v>
@@ -3220,10 +3220,10 @@
         <v>4</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E134" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H134" s="3">
         <v>1</v>
@@ -3246,7 +3246,7 @@
         <v>5</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E135" s="3"/>
       <c r="H135" s="3">
@@ -3270,7 +3270,7 @@
         <v>5</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E136" s="3"/>
       <c r="H136" s="3">
@@ -3294,7 +3294,7 @@
         <v>5</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E137" s="3"/>
       <c r="H137" s="3">
@@ -3318,10 +3318,10 @@
         <v>6</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E138" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H138" s="3">
         <v>1</v>
@@ -3344,10 +3344,10 @@
         <v>6</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E139" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H139" s="3">
         <v>1</v>
@@ -3370,10 +3370,10 @@
         <v>6</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E140" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H140" s="3">
         <v>1</v>
@@ -3396,7 +3396,7 @@
         <v>7</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E141" s="3"/>
       <c r="H141" s="3">
@@ -3420,7 +3420,7 @@
         <v>7</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E142" s="3"/>
       <c r="H142" s="3">
@@ -3444,7 +3444,7 @@
         <v>7</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E143" s="3"/>
       <c r="H143" s="3">
@@ -3468,10 +3468,10 @@
         <v>8</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E144" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H144" s="3">
         <v>1</v>
@@ -3494,10 +3494,10 @@
         <v>8</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E145" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H145" s="3">
         <v>1</v>
@@ -3520,10 +3520,10 @@
         <v>8</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E146" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H146" s="3">
         <v>1</v>
@@ -3546,7 +3546,7 @@
         <v>1</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E147" s="3"/>
       <c r="G147">
@@ -3573,7 +3573,7 @@
         <v>1</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E148" s="3"/>
       <c r="G148">
@@ -3600,7 +3600,7 @@
         <v>1</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E149" s="3"/>
       <c r="G149">
@@ -3627,10 +3627,10 @@
         <v>2</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E150" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G150">
         <v>25.4</v>
@@ -3656,10 +3656,10 @@
         <v>2</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E151" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G151">
         <v>25.6</v>
@@ -3685,10 +3685,10 @@
         <v>2</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E152" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G152">
         <v>24.5</v>
@@ -3714,10 +3714,10 @@
         <v>2</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E153" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H153" s="3">
         <v>2</v>
@@ -3740,7 +3740,7 @@
         <v>3</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E154" s="3"/>
       <c r="G154">
@@ -3767,7 +3767,7 @@
         <v>3</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E155" s="3"/>
       <c r="G155">
@@ -3794,7 +3794,7 @@
         <v>3</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E156" s="3"/>
       <c r="G156">
@@ -3821,10 +3821,10 @@
         <v>4</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E157" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G157">
         <v>23.7</v>
@@ -3850,10 +3850,10 @@
         <v>4</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E158" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G158">
         <v>25.2</v>
@@ -3879,10 +3879,10 @@
         <v>4</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E159" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G159">
         <v>24.6</v>
@@ -3908,7 +3908,7 @@
         <v>5</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E160" s="3"/>
       <c r="G160">
@@ -3935,7 +3935,7 @@
         <v>5</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E161" s="3"/>
       <c r="G161">
@@ -3962,7 +3962,7 @@
         <v>5</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E162" s="3"/>
       <c r="G162">
@@ -3989,10 +3989,10 @@
         <v>6</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E163" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G163">
         <v>24.6</v>
@@ -4018,10 +4018,10 @@
         <v>6</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E164" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H164" s="3">
         <v>2</v>
@@ -4044,10 +4044,10 @@
         <v>6</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E165" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G165">
         <v>24.4</v>
@@ -4073,10 +4073,10 @@
         <v>6</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E166" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H166" s="3">
         <v>2</v>
@@ -4099,10 +4099,10 @@
         <v>6</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E167" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G167">
         <v>23.6</v>
@@ -4128,7 +4128,7 @@
         <v>7</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E168" s="3"/>
       <c r="G168">
@@ -4155,7 +4155,7 @@
         <v>7</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E169" s="3"/>
       <c r="G169">
@@ -4182,7 +4182,7 @@
         <v>7</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E170" s="3"/>
       <c r="G170">
@@ -4209,10 +4209,10 @@
         <v>8</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E171" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G171">
         <v>25.5</v>
@@ -4238,10 +4238,10 @@
         <v>8</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E172" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G172">
         <v>25</v>
@@ -4267,10 +4267,10 @@
         <v>8</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E173" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G173">
         <v>26.4</v>
@@ -4296,7 +4296,7 @@
         <v>1</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E174" s="3"/>
       <c r="H174" s="3">
@@ -4320,7 +4320,7 @@
         <v>1</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E175" s="3"/>
       <c r="H175" s="3">
@@ -4344,7 +4344,7 @@
         <v>1</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E176" s="3"/>
       <c r="H176" s="3">
@@ -4368,10 +4368,10 @@
         <v>2</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E177" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H177" s="3">
         <v>1</v>
@@ -4394,10 +4394,10 @@
         <v>2</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E178" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H178" s="3">
         <v>1</v>
@@ -4420,10 +4420,10 @@
         <v>2</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E179" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H179" s="3">
         <v>1</v>
@@ -4446,10 +4446,10 @@
         <v>2</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E180" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H180" s="3">
         <v>2</v>
@@ -4472,7 +4472,7 @@
         <v>3</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E181" s="3"/>
       <c r="H181" s="3">
@@ -4496,7 +4496,7 @@
         <v>3</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E182" s="3"/>
       <c r="H182" s="3">
@@ -4520,7 +4520,7 @@
         <v>3</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E183" s="3"/>
       <c r="H183" s="3">
@@ -4544,10 +4544,10 @@
         <v>4</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E184" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H184" s="3">
         <v>1</v>
@@ -4570,10 +4570,10 @@
         <v>4</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E185" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H185" s="3">
         <v>1</v>
@@ -4596,10 +4596,10 @@
         <v>4</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E186" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H186" s="3">
         <v>1</v>
@@ -4622,7 +4622,7 @@
         <v>5</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E187" s="3"/>
       <c r="H187" s="3">
@@ -4646,7 +4646,7 @@
         <v>5</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E188" s="3"/>
       <c r="H188" s="3">
@@ -4670,7 +4670,7 @@
         <v>5</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E189" s="3"/>
       <c r="H189" s="3">
@@ -4694,10 +4694,10 @@
         <v>6</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E190" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H190" s="3">
         <v>1</v>
@@ -4720,10 +4720,10 @@
         <v>6</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E191" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H191" s="3">
         <v>2</v>
@@ -4746,10 +4746,10 @@
         <v>6</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E192" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H192" s="3">
         <v>1</v>
@@ -4772,10 +4772,10 @@
         <v>6</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E193" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H193" s="3">
         <v>2</v>
@@ -4798,10 +4798,10 @@
         <v>6</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E194" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H194" s="3">
         <v>1</v>
@@ -4824,7 +4824,7 @@
         <v>7</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E195" s="3"/>
       <c r="H195" s="3">
@@ -4848,7 +4848,7 @@
         <v>7</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E196" s="3"/>
       <c r="H196" s="3">
@@ -4872,7 +4872,7 @@
         <v>7</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E197" s="3"/>
       <c r="H197" s="3">
@@ -4896,10 +4896,10 @@
         <v>8</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E198" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H198" s="3">
         <v>1</v>
@@ -4922,10 +4922,10 @@
         <v>8</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E199" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H199" s="3">
         <v>1</v>
@@ -4948,10 +4948,10 @@
         <v>8</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E200" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H200" s="3">
         <v>1</v>
@@ -4961,6 +4961,1368 @@
       </c>
       <c r="J200" s="3">
         <v>4.7</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B201" s="3">
+        <v>1</v>
+      </c>
+      <c r="C201" s="3">
+        <v>1</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E201" s="3"/>
+      <c r="H201" s="3">
+        <v>1</v>
+      </c>
+      <c r="I201" s="3">
+        <v>9.6</v>
+      </c>
+      <c r="J201" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B202" s="3">
+        <v>2</v>
+      </c>
+      <c r="C202" s="3">
+        <v>1</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E202" s="3"/>
+      <c r="H202" s="3">
+        <v>1</v>
+      </c>
+      <c r="I202" s="3">
+        <v>13.1</v>
+      </c>
+      <c r="J202" s="3">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B203" s="3">
+        <v>3</v>
+      </c>
+      <c r="C203" s="3">
+        <v>1</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E203" s="3"/>
+      <c r="H203" s="3">
+        <v>1</v>
+      </c>
+      <c r="I203" s="3">
+        <v>13</v>
+      </c>
+      <c r="J203" s="3">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B204" s="3">
+        <v>1</v>
+      </c>
+      <c r="C204" s="3">
+        <v>2</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E204" t="s">
+        <v>9</v>
+      </c>
+      <c r="H204" s="3">
+        <v>1</v>
+      </c>
+      <c r="I204" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="J204" s="3">
+        <v>5.6</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B205" s="3">
+        <v>2</v>
+      </c>
+      <c r="C205" s="3">
+        <v>2</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E205" t="s">
+        <v>9</v>
+      </c>
+      <c r="H205" s="3">
+        <v>1</v>
+      </c>
+      <c r="I205" s="3">
+        <v>9.6</v>
+      </c>
+      <c r="J205" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B206" s="3">
+        <v>3</v>
+      </c>
+      <c r="C206" s="3">
+        <v>2</v>
+      </c>
+      <c r="D206" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E206" t="s">
+        <v>9</v>
+      </c>
+      <c r="H206" s="3">
+        <v>1</v>
+      </c>
+      <c r="I206" s="3">
+        <v>6.3</v>
+      </c>
+      <c r="J206" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B207" s="3">
+        <v>1</v>
+      </c>
+      <c r="C207" s="3">
+        <v>3</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E207" s="3"/>
+      <c r="H207" s="3">
+        <v>1</v>
+      </c>
+      <c r="I207" s="3">
+        <v>11.6</v>
+      </c>
+      <c r="J207" s="3">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B208" s="3">
+        <v>2</v>
+      </c>
+      <c r="C208" s="3">
+        <v>3</v>
+      </c>
+      <c r="D208" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E208" s="3"/>
+      <c r="H208" s="3">
+        <v>1</v>
+      </c>
+      <c r="I208" s="3">
+        <v>8.1</v>
+      </c>
+      <c r="J208" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B209" s="3">
+        <v>3</v>
+      </c>
+      <c r="C209" s="3">
+        <v>3</v>
+      </c>
+      <c r="D209" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E209" s="3"/>
+      <c r="H209" s="3">
+        <v>1</v>
+      </c>
+      <c r="I209" s="3">
+        <v>10.1</v>
+      </c>
+      <c r="J209" s="3">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A210" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B210" s="3">
+        <v>1</v>
+      </c>
+      <c r="C210" s="3">
+        <v>4</v>
+      </c>
+      <c r="D210" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E210" t="s">
+        <v>9</v>
+      </c>
+      <c r="H210" s="3">
+        <v>1</v>
+      </c>
+      <c r="I210" s="3">
+        <v>6.3</v>
+      </c>
+      <c r="J210" s="3">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A211" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B211" s="3">
+        <v>2</v>
+      </c>
+      <c r="C211" s="3">
+        <v>4</v>
+      </c>
+      <c r="D211" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E211" t="s">
+        <v>9</v>
+      </c>
+      <c r="H211" s="3">
+        <v>1</v>
+      </c>
+      <c r="I211" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="J211" s="3">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B212" s="3">
+        <v>3</v>
+      </c>
+      <c r="C212" s="3">
+        <v>4</v>
+      </c>
+      <c r="D212" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E212" t="s">
+        <v>9</v>
+      </c>
+      <c r="H212" s="3">
+        <v>1</v>
+      </c>
+      <c r="I212" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="J212" s="3">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A213" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B213" s="3">
+        <v>1</v>
+      </c>
+      <c r="C213" s="3">
+        <v>5</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E213" s="3"/>
+      <c r="H213" s="3">
+        <v>1</v>
+      </c>
+      <c r="I213" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="J213" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B214" s="3">
+        <v>2</v>
+      </c>
+      <c r="C214" s="3">
+        <v>5</v>
+      </c>
+      <c r="D214" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E214" s="3"/>
+      <c r="H214" s="3">
+        <v>1</v>
+      </c>
+      <c r="I214" s="3">
+        <v>13.3</v>
+      </c>
+      <c r="J214" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B215" s="3">
+        <v>3</v>
+      </c>
+      <c r="C215" s="3">
+        <v>5</v>
+      </c>
+      <c r="D215" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E215" s="3"/>
+      <c r="H215" s="3">
+        <v>1</v>
+      </c>
+      <c r="I215" s="3">
+        <v>11.8</v>
+      </c>
+      <c r="J215" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A216" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B216" s="3">
+        <v>1</v>
+      </c>
+      <c r="C216" s="3">
+        <v>6</v>
+      </c>
+      <c r="D216" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E216" t="s">
+        <v>9</v>
+      </c>
+      <c r="H216" s="3">
+        <v>1</v>
+      </c>
+      <c r="I216" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="J216" s="3">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A217" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B217" s="3">
+        <v>2</v>
+      </c>
+      <c r="C217" s="3">
+        <v>6</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E217" t="s">
+        <v>9</v>
+      </c>
+      <c r="H217" s="3">
+        <v>1</v>
+      </c>
+      <c r="I217" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="J217" s="3">
+        <v>10.4</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A218" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B218" s="3">
+        <v>3</v>
+      </c>
+      <c r="C218" s="3">
+        <v>6</v>
+      </c>
+      <c r="D218" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E218" t="s">
+        <v>9</v>
+      </c>
+      <c r="H218" s="3">
+        <v>1</v>
+      </c>
+      <c r="I218" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="J218" s="3">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A219" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B219" s="3">
+        <v>1</v>
+      </c>
+      <c r="C219" s="3">
+        <v>7</v>
+      </c>
+      <c r="D219" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E219" s="3"/>
+      <c r="H219" s="3">
+        <v>1</v>
+      </c>
+      <c r="I219" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="J219" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A220" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B220" s="3">
+        <v>2</v>
+      </c>
+      <c r="C220" s="3">
+        <v>7</v>
+      </c>
+      <c r="D220" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E220" s="3"/>
+      <c r="H220" s="3">
+        <v>1</v>
+      </c>
+      <c r="I220" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="J220" s="3">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B221" s="3">
+        <v>3</v>
+      </c>
+      <c r="C221" s="3">
+        <v>7</v>
+      </c>
+      <c r="D221" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E221" s="3"/>
+      <c r="H221" s="3">
+        <v>1</v>
+      </c>
+      <c r="I221" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="J221" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A222" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B222" s="3">
+        <v>1</v>
+      </c>
+      <c r="C222" s="3">
+        <v>8</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E222" t="s">
+        <v>9</v>
+      </c>
+      <c r="H222" s="3">
+        <v>1</v>
+      </c>
+      <c r="I222" s="3">
+        <v>9.9</v>
+      </c>
+      <c r="J222" s="3">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B223" s="3">
+        <v>2</v>
+      </c>
+      <c r="C223" s="3">
+        <v>8</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E223" t="s">
+        <v>9</v>
+      </c>
+      <c r="H223" s="3">
+        <v>1</v>
+      </c>
+      <c r="I223" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="J223">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A224" s="1">
+        <v>44906</v>
+      </c>
+      <c r="B224" s="3">
+        <v>3</v>
+      </c>
+      <c r="C224" s="3">
+        <v>8</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E224" t="s">
+        <v>9</v>
+      </c>
+      <c r="H224" s="3">
+        <v>1</v>
+      </c>
+      <c r="I224">
+        <v>11.9</v>
+      </c>
+      <c r="J224">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A225" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B225" s="3">
+        <v>1</v>
+      </c>
+      <c r="C225" s="3">
+        <v>1</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E225" s="3"/>
+      <c r="G225">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="H225" s="3">
+        <v>1</v>
+      </c>
+      <c r="I225" s="3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J225" s="3">
+        <v>7.7</v>
+      </c>
+      <c r="K225" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A226" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B226" s="3">
+        <v>2</v>
+      </c>
+      <c r="C226" s="3">
+        <v>1</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E226" s="3"/>
+      <c r="G226">
+        <v>25.9</v>
+      </c>
+      <c r="H226" s="3">
+        <v>1</v>
+      </c>
+      <c r="I226" s="3">
+        <v>15.9</v>
+      </c>
+      <c r="J226" s="3">
+        <v>9</v>
+      </c>
+      <c r="K226" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A227" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B227" s="3">
+        <v>3</v>
+      </c>
+      <c r="C227" s="3">
+        <v>1</v>
+      </c>
+      <c r="D227" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E227" s="3"/>
+      <c r="G227">
+        <v>25.1</v>
+      </c>
+      <c r="H227" s="3">
+        <v>1</v>
+      </c>
+      <c r="I227" s="3">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="J227" s="3">
+        <v>15.2</v>
+      </c>
+      <c r="K227" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A228" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B228" s="3">
+        <v>1</v>
+      </c>
+      <c r="C228" s="3">
+        <v>2</v>
+      </c>
+      <c r="D228" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E228" t="s">
+        <v>9</v>
+      </c>
+      <c r="G228">
+        <v>25.7</v>
+      </c>
+      <c r="H228" s="3">
+        <v>1</v>
+      </c>
+      <c r="I228" s="3">
+        <v>9.5</v>
+      </c>
+      <c r="J228" s="3">
+        <v>8.1</v>
+      </c>
+      <c r="K228" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A229" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B229" s="3">
+        <v>2</v>
+      </c>
+      <c r="C229" s="3">
+        <v>2</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E229" t="s">
+        <v>9</v>
+      </c>
+      <c r="G229">
+        <v>25.7</v>
+      </c>
+      <c r="H229" s="3">
+        <v>1</v>
+      </c>
+      <c r="I229" s="3">
+        <v>11.8</v>
+      </c>
+      <c r="J229" s="3">
+        <v>6.9</v>
+      </c>
+      <c r="K229" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A230" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B230" s="3">
+        <v>3</v>
+      </c>
+      <c r="C230" s="3">
+        <v>2</v>
+      </c>
+      <c r="D230" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E230" t="s">
+        <v>9</v>
+      </c>
+      <c r="G230">
+        <v>25.9</v>
+      </c>
+      <c r="H230" s="3">
+        <v>1</v>
+      </c>
+      <c r="I230" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="J230" s="3">
+        <v>6.8</v>
+      </c>
+      <c r="K230" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A231" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B231" s="3">
+        <v>1</v>
+      </c>
+      <c r="C231" s="3">
+        <v>3</v>
+      </c>
+      <c r="D231" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E231" s="3"/>
+      <c r="G231">
+        <v>26.4</v>
+      </c>
+      <c r="H231" s="3">
+        <v>1</v>
+      </c>
+      <c r="I231" s="3">
+        <v>10.9</v>
+      </c>
+      <c r="J231" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K231" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A232" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B232" s="3">
+        <v>2</v>
+      </c>
+      <c r="C232" s="3">
+        <v>3</v>
+      </c>
+      <c r="D232" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E232" s="3"/>
+      <c r="G232">
+        <v>24.1</v>
+      </c>
+      <c r="H232" s="3">
+        <v>1</v>
+      </c>
+      <c r="I232" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J232" s="3">
+        <v>6.9</v>
+      </c>
+      <c r="K232" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A233" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B233" s="3">
+        <v>3</v>
+      </c>
+      <c r="C233" s="3">
+        <v>3</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E233" s="3"/>
+      <c r="G233">
+        <v>24.2</v>
+      </c>
+      <c r="H233" s="3">
+        <v>1</v>
+      </c>
+      <c r="I233" s="3">
+        <v>14.6</v>
+      </c>
+      <c r="J233" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="K233" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A234" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B234" s="3">
+        <v>1</v>
+      </c>
+      <c r="C234" s="3">
+        <v>4</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E234" t="s">
+        <v>9</v>
+      </c>
+      <c r="G234">
+        <v>23.9</v>
+      </c>
+      <c r="H234" s="3">
+        <v>1</v>
+      </c>
+      <c r="I234" s="3">
+        <v>8</v>
+      </c>
+      <c r="J234" s="3">
+        <v>7.1</v>
+      </c>
+      <c r="K234" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A235" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B235" s="3">
+        <v>2</v>
+      </c>
+      <c r="C235" s="3">
+        <v>4</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E235" t="s">
+        <v>9</v>
+      </c>
+      <c r="G235">
+        <v>25.2</v>
+      </c>
+      <c r="H235" s="3">
+        <v>1</v>
+      </c>
+      <c r="I235" s="3">
+        <v>9</v>
+      </c>
+      <c r="J235" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="K235" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A236" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B236" s="3">
+        <v>3</v>
+      </c>
+      <c r="C236" s="3">
+        <v>4</v>
+      </c>
+      <c r="D236" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E236" t="s">
+        <v>9</v>
+      </c>
+      <c r="G236">
+        <v>25.2</v>
+      </c>
+      <c r="H236" s="3">
+        <v>1</v>
+      </c>
+      <c r="I236" s="3">
+        <v>13.3</v>
+      </c>
+      <c r="J236" s="3">
+        <v>8</v>
+      </c>
+      <c r="K236" s="3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A237" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B237" s="3">
+        <v>1</v>
+      </c>
+      <c r="C237" s="3">
+        <v>5</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E237" s="3"/>
+      <c r="G237">
+        <v>23.6</v>
+      </c>
+      <c r="H237" s="3">
+        <v>1</v>
+      </c>
+      <c r="I237" s="3">
+        <v>9.4</v>
+      </c>
+      <c r="J237" s="3">
+        <v>6.8</v>
+      </c>
+      <c r="K237" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A238" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B238" s="3"/>
+      <c r="C238" s="3"/>
+      <c r="D238" s="3"/>
+      <c r="E238" s="3"/>
+      <c r="H238" s="3">
+        <v>2</v>
+      </c>
+      <c r="I238" s="3">
+        <v>6.8</v>
+      </c>
+      <c r="J238" s="3">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A239" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B239" s="3">
+        <v>2</v>
+      </c>
+      <c r="C239" s="3">
+        <v>5</v>
+      </c>
+      <c r="D239" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E239" s="3"/>
+      <c r="G239">
+        <v>26.4</v>
+      </c>
+      <c r="H239" s="3">
+        <v>1</v>
+      </c>
+      <c r="I239" s="3">
+        <v>17.5</v>
+      </c>
+      <c r="J239" s="3">
+        <v>11.4</v>
+      </c>
+      <c r="K239" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A240" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B240" s="3">
+        <v>3</v>
+      </c>
+      <c r="C240" s="3">
+        <v>5</v>
+      </c>
+      <c r="D240" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E240" s="3"/>
+      <c r="G240">
+        <v>25.5</v>
+      </c>
+      <c r="H240" s="3">
+        <v>1</v>
+      </c>
+      <c r="I240" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="J240" s="3">
+        <v>12</v>
+      </c>
+      <c r="K240" s="3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B241" s="3">
+        <v>1</v>
+      </c>
+      <c r="C241" s="3">
+        <v>6</v>
+      </c>
+      <c r="D241" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E241" t="s">
+        <v>9</v>
+      </c>
+      <c r="G241">
+        <v>25.4</v>
+      </c>
+      <c r="H241" s="3">
+        <v>1</v>
+      </c>
+      <c r="I241" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="J241" s="3">
+        <v>5.3</v>
+      </c>
+      <c r="K241" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B242" s="3">
+        <v>2</v>
+      </c>
+      <c r="C242" s="3">
+        <v>6</v>
+      </c>
+      <c r="D242" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E242" t="s">
+        <v>9</v>
+      </c>
+      <c r="G242">
+        <v>24.6</v>
+      </c>
+      <c r="H242" s="3">
+        <v>1</v>
+      </c>
+      <c r="I242" s="3">
+        <v>13.3</v>
+      </c>
+      <c r="J242" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="K242" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B243" s="3">
+        <v>3</v>
+      </c>
+      <c r="C243" s="3">
+        <v>6</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E243" t="s">
+        <v>9</v>
+      </c>
+      <c r="G243">
+        <v>25</v>
+      </c>
+      <c r="H243" s="3">
+        <v>1</v>
+      </c>
+      <c r="I243" s="3">
+        <v>10.9</v>
+      </c>
+      <c r="J243" s="3">
+        <v>7.3</v>
+      </c>
+      <c r="K243" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A244" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B244" s="3">
+        <v>1</v>
+      </c>
+      <c r="C244" s="3">
+        <v>7</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E244" s="3"/>
+      <c r="G244">
+        <v>24.5</v>
+      </c>
+      <c r="H244" s="3">
+        <v>1</v>
+      </c>
+      <c r="I244" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="J244" s="3">
+        <v>4</v>
+      </c>
+      <c r="K244" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A245" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B245" s="3">
+        <v>2</v>
+      </c>
+      <c r="C245" s="3">
+        <v>7</v>
+      </c>
+      <c r="D245" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E245" s="3"/>
+      <c r="G245">
+        <v>26</v>
+      </c>
+      <c r="H245" s="3">
+        <v>1</v>
+      </c>
+      <c r="I245" s="3">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="J245" s="3">
+        <v>6.2</v>
+      </c>
+      <c r="K245" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B246" s="3">
+        <v>3</v>
+      </c>
+      <c r="C246" s="3">
+        <v>7</v>
+      </c>
+      <c r="D246" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E246" s="3"/>
+      <c r="G246">
+        <v>26.8</v>
+      </c>
+      <c r="H246" s="3">
+        <v>1</v>
+      </c>
+      <c r="I246" s="3">
+        <v>0</v>
+      </c>
+      <c r="J246" s="3">
+        <v>0</v>
+      </c>
+      <c r="K246" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A247" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B247" s="3">
+        <v>1</v>
+      </c>
+      <c r="C247" s="3">
+        <v>8</v>
+      </c>
+      <c r="D247" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E247" t="s">
+        <v>9</v>
+      </c>
+      <c r="G247">
+        <v>26.6</v>
+      </c>
+      <c r="H247" s="3">
+        <v>1</v>
+      </c>
+      <c r="I247" s="3">
+        <v>11.8</v>
+      </c>
+      <c r="J247" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="K247" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B248" s="3">
+        <v>2</v>
+      </c>
+      <c r="C248" s="3">
+        <v>8</v>
+      </c>
+      <c r="D248" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E248" t="s">
+        <v>9</v>
+      </c>
+      <c r="G248">
+        <v>25.8</v>
+      </c>
+      <c r="H248" s="3">
+        <v>1</v>
+      </c>
+      <c r="I248" s="3">
+        <v>15.4</v>
+      </c>
+      <c r="J248" s="3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="K248" s="3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A249" s="1">
+        <v>44909</v>
+      </c>
+      <c r="B249" s="3">
+        <v>3</v>
+      </c>
+      <c r="C249" s="3">
+        <v>8</v>
+      </c>
+      <c r="D249" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E249" t="s">
+        <v>9</v>
+      </c>
+      <c r="G249">
+        <v>25.7</v>
+      </c>
+      <c r="H249" s="3">
+        <v>1</v>
+      </c>
+      <c r="I249" s="3">
+        <v>11.9</v>
+      </c>
+      <c r="J249" s="3">
+        <v>8.1</v>
+      </c>
+      <c r="K249" s="3">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>